<commit_message>
La in noen figurer
</commit_message>
<xml_diff>
--- a/Lab2/Resukltater.xlsx
+++ b/Lab2/Resukltater.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marku\Documents\TTT4280\Lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B397101-0D8F-4B3B-A217-9D68A106E277}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C41E0C3-E417-4CAD-B0C1-EB28DDC8300D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4C115540-8A80-43B9-A406-FC39B108DFD0}"/>
   </bookViews>
@@ -30,14 +30,10 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -70,7 +66,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,7 +384,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>